<commit_message>
changed adverse events file
</commit_message>
<xml_diff>
--- a/results_adverse-events.v2.0.xlsx
+++ b/results_adverse-events.v2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jottacloud\PDtremor_syst-review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE439B38-A295-4266-8759-FA6EA284A191}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125B3B5-CC55-42E9-A750-94A8E8D00169}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="133">
   <si>
     <t>slab</t>
   </si>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2495,11 +2495,11 @@
       <c r="C29" t="s">
         <v>27</v>
       </c>
-      <c r="D29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" t="s">
-        <v>131</v>
+      <c r="D29">
+        <v>27</v>
+      </c>
+      <c r="E29">
+        <v>18</v>
       </c>
       <c r="F29" t="s">
         <v>131</v>

</xml_diff>